<commit_message>
update:     sql file     draw.io file     xlsx files fix:     rename package     rename files     add libs losing
</commit_message>
<xml_diff>
--- a/Từ điển dữ liệu.xlsx
+++ b/Từ điển dữ liệu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/746813123f077acb/Máy tính/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="493" documentId="13_ncr:1_{0E6CEDA0-CCDF-4949-A372-F8E2A066A992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F54F3B3C-6F9D-4119-AD00-48B31349B93F}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="13_ncr:1_{0E6CEDA0-CCDF-4949-A372-F8E2A066A992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E4F3228-7D96-4EA2-A86C-A77C4DD7A9C8}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="75" windowWidth="14205" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="14205" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Từ điển tổng hợp" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="215">
   <si>
     <t>STT</t>
   </si>
@@ -442,9 +442,6 @@
     <t>1' - nam, '0' - nữ, 'null' - không xác định.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Buộc xóa bảng khóa ngoại khi xóa bảng.</t>
-  </si>
-  <si>
     <t>Ít nhất 18 tuổi.</t>
   </si>
   <si>
@@ -541,9 +538,6 @@
     <t>IdGV_GiangDay</t>
   </si>
   <si>
-    <t>MuonPhongHoc</t>
-  </si>
-  <si>
     <t>IdTaiKhoan_MPH</t>
   </si>
   <si>
@@ -604,12 +598,6 @@
     <t>Thời điểm hủy áp dụng (hủy tài khoản)</t>
   </si>
   <si>
-    <t>IdMPH</t>
-  </si>
-  <si>
-    <t>Id mượn phòng học</t>
-  </si>
-  <si>
     <t>Ngay_BD</t>
   </si>
   <si>
@@ -677,6 +665,27 @@
   </si>
   <si>
     <t>LichMuonPhong</t>
+  </si>
+  <si>
+    <t>Mục đích mượn phòng học</t>
+  </si>
+  <si>
+    <t>MucDich</t>
+  </si>
+  <si>
+    <t>YeuCauHocCu</t>
+  </si>
+  <si>
+    <t>Yêu cầu mượn học cụ</t>
+  </si>
+  <si>
+    <t>ThoiGian_MPH</t>
+  </si>
+  <si>
+    <t>Thời gian mượn phòng học</t>
+  </si>
+  <si>
+    <t>Lý do thay đổi lịch học hoặc tạo lich mượn phòng</t>
   </si>
 </sst>
 </file>
@@ -911,10 +920,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1200,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C14DD0-095C-497D-B714-923494B6BFAC}">
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1218,14 +1227,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="29"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
@@ -1243,13 +1252,13 @@
         <v>131</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1257,19 +1266,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -1278,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="10" t="str">
         <f>C60</f>
@@ -1302,20 +1311,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>138</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1326,14 +1335,14 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -1342,20 +1351,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1363,10 +1372,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
@@ -1382,10 +1391,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1399,15 +1408,15 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -1420,14 +1429,14 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
@@ -1445,13 +1454,13 @@
         <v>131</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1459,19 +1468,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -1480,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" s="10" t="str">
         <f>C3</f>
@@ -1531,7 +1540,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
@@ -1550,7 +1559,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="27"/>
@@ -1558,7 +1567,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
@@ -1569,7 +1578,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="27"/>
@@ -1588,7 +1597,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1622,7 +1631,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
@@ -1636,15 +1645,15 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -1657,14 +1666,14 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
@@ -1682,13 +1691,13 @@
         <v>131</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1696,19 +1705,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G27" s="10"/>
     </row>
@@ -1717,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" s="10" t="str">
         <f>C3</f>
@@ -1744,7 +1753,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10" t="s">
@@ -1763,7 +1772,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="27"/>
@@ -1771,7 +1780,7 @@
         <v>31</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
@@ -1782,7 +1791,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="27"/>
@@ -1801,12 +1810,12 @@
         <v>8</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -1835,7 +1844,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
@@ -1849,15 +1858,15 @@
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -1870,14 +1879,14 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="30"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="7"/>
       <c r="F37" s="17"/>
     </row>
@@ -1895,13 +1904,13 @@
         <v>131</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1912,13 +1921,13 @@
         <v>110</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>118</v>
@@ -1930,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="10" t="str">
         <f>C3</f>
@@ -1957,7 +1966,7 @@
         <v>24</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>16</v>
@@ -1975,14 +1984,14 @@
         <v>25</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D42" s="10"/>
       <c r="F42" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
@@ -1993,7 +2002,7 @@
         <v>26</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="27"/>
@@ -2012,12 +2021,12 @@
         <v>8</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G44" s="10"/>
     </row>
@@ -2049,14 +2058,14 @@
       <c r="K46" s="26"/>
     </row>
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="29"/>
       <c r="E47" s="7"/>
       <c r="F47" s="17"/>
     </row>
@@ -2074,13 +2083,13 @@
         <v>131</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -2088,19 +2097,19 @@
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G49" s="10"/>
     </row>
@@ -2109,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C50" s="10" t="str">
         <f>C3</f>
@@ -2127,7 +2136,7 @@
         <v>Id tài khoản</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
@@ -2135,7 +2144,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C51" s="10" t="str">
         <f>C39</f>
@@ -2159,15 +2168,15 @@
         <v>4</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D52" s="27"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G52" s="10"/>
     </row>
@@ -2179,14 +2188,14 @@
         <v>75</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G53" s="10"/>
     </row>
@@ -2195,10 +2204,10 @@
         <v>6</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10" t="s">
@@ -2214,15 +2223,15 @@
         <v>7</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G55" s="10"/>
     </row>
@@ -2231,17 +2240,17 @@
         <v>8</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G56" s="10"/>
       <c r="K56" s="26"/>
@@ -2255,14 +2264,14 @@
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="D58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="29"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
     </row>
@@ -2280,13 +2289,13 @@
         <v>131</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -2294,19 +2303,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G60" s="10"/>
     </row>
@@ -2315,10 +2324,10 @@
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10" t="s">
@@ -2328,7 +2337,7 @@
         <v>43</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2340,14 +2349,14 @@
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="D63" s="30"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D63" s="29"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
     </row>
@@ -2365,13 +2374,13 @@
         <v>131</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -2382,13 +2391,13 @@
         <v>100</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>101</v>
@@ -2400,10 +2409,10 @@
         <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="10" t="s">
@@ -2415,14 +2424,14 @@
       <c r="G66" s="10"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="29"/>
-      <c r="C68" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="D68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D68" s="29"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
@@ -2440,13 +2449,13 @@
         <v>131</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="57" x14ac:dyDescent="0.2">
@@ -2465,7 +2474,7 @@
         <v>Primary key, Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F70" s="10" t="str">
         <f>F83</f>
@@ -2478,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C71" s="10" t="str">
         <f>C3</f>
@@ -2489,7 +2498,7 @@
         <v>Primary key, Foreign key (TaiKhoan - IdTaiKhoan)</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F71" s="10" t="str">
         <f>_xlfn.CONCAT(F3, " (Tài khoản mượn phòng)")</f>
@@ -2502,10 +2511,10 @@
         <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="10" t="s">
@@ -2525,14 +2534,14 @@
       <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="29"/>
-      <c r="C74" s="30" t="s">
+      <c r="B74" s="30"/>
+      <c r="C74" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D74" s="30"/>
+      <c r="D74" s="29"/>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
     </row>
@@ -2550,13 +2559,13 @@
         <v>131</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -2567,13 +2576,13 @@
         <v>49</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>52</v>
@@ -2588,7 +2597,7 @@
         <v>50</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D77" s="27"/>
       <c r="E77" s="10" t="s">
@@ -2604,10 +2613,10 @@
         <v>3</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>16</v>
@@ -2622,15 +2631,15 @@
         <v>4</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D79" s="10"/>
       <c r="E79" s="10"/>
       <c r="F79" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G79" s="10"/>
     </row>
@@ -2643,14 +2652,14 @@
       <c r="F80" s="7"/>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="29"/>
-      <c r="C81" s="30" t="s">
+      <c r="B81" s="30"/>
+      <c r="C81" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="30"/>
+      <c r="D81" s="29"/>
       <c r="E81" s="17"/>
       <c r="F81" s="17"/>
     </row>
@@ -2668,13 +2677,13 @@
         <v>131</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -2685,13 +2694,13 @@
         <v>54</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>55</v>
@@ -2703,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C84" s="10" t="str">
         <f>C3</f>
@@ -2714,7 +2723,7 @@
         <v>Foreign key (GiangVien - IdGV)</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F84" s="10" t="str">
         <f>_xlfn.CONCAT(F27, " (Giảng viên giảng dạy)")</f>
@@ -2775,15 +2784,15 @@
         <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
       <c r="F87" s="10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G87" s="10"/>
     </row>
@@ -2792,15 +2801,15 @@
         <v>6</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D88" s="10"/>
       <c r="E88" s="10"/>
       <c r="F88" s="10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G88" s="10"/>
     </row>
@@ -2809,10 +2818,10 @@
         <v>7</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D89" s="27"/>
       <c r="E89" s="10" t="s">
@@ -2828,15 +2837,15 @@
         <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D90" s="10"/>
       <c r="E90" s="10"/>
       <c r="F90" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G90" s="10"/>
     </row>
@@ -2849,14 +2858,14 @@
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="29" t="s">
+      <c r="A92" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B92" s="29"/>
-      <c r="C92" s="30" t="s">
+      <c r="B92" s="30"/>
+      <c r="C92" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D92" s="30"/>
+      <c r="D92" s="29"/>
       <c r="E92" s="22"/>
       <c r="F92" s="22"/>
     </row>
@@ -2874,13 +2883,13 @@
         <v>131</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F93" s="12" t="s">
         <v>119</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -2891,13 +2900,13 @@
         <v>58</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>65</v>
@@ -2912,7 +2921,7 @@
         <v>69</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D95" s="27"/>
       <c r="E95" s="10" t="s">
@@ -2928,10 +2937,10 @@
         <v>3</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>16</v>
@@ -2946,15 +2955,15 @@
         <v>4</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
       <c r="F97" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G97" s="10"/>
     </row>
@@ -2967,12 +2976,12 @@
       <c r="F98" s="7"/>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B99" s="29"/>
+      <c r="B99" s="30"/>
       <c r="C99" s="31" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="D99" s="31"/>
       <c r="E99" s="22"/>
@@ -2992,13 +3001,13 @@
         <v>131</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F100" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -3006,19 +3015,19 @@
         <v>1</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E101" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>188</v>
+        <v>96</v>
       </c>
       <c r="G101" s="10"/>
     </row>
@@ -3027,21 +3036,21 @@
         <v>2</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
       <c r="C102" s="10" t="str">
-        <f>C3</f>
-        <v>unique identifier</v>
+        <f>C83</f>
+        <v>varchar(15)</v>
       </c>
       <c r="D102" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (",C1, " - ", B3,")")</f>
-        <v>Foreign key (TaiKhoan - IdTaiKhoan)</v>
+        <f>_xlfn.CONCAT( "Foreign key (", C81, " - ", B83,")")</f>
+        <v>Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>130</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
       <c r="G102" s="10"/>
     </row>
@@ -3050,311 +3059,223 @@
         <v>3</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>168</v>
+        <v>58</v>
       </c>
       <c r="C103" s="10" t="str">
-        <f>C39</f>
+        <f>C94</f>
+        <v>varchar(10)</v>
+      </c>
+      <c r="D103" s="10" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (", C92, " - ", B94,")")</f>
+        <v>Foreign key (PhongHoc - MaPH)</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F103" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A104" s="23">
+        <v>5</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C104" s="10" t="str">
+        <f>C14</f>
         <v>unique identifier</v>
       </c>
-      <c r="D103" s="10" t="str">
+      <c r="D104" s="10" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (",C1, " - ", B3,")")</f>
+        <v>Foreign key (TaiKhoan - IdTaiKhoan)</v>
+      </c>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A105" s="23">
+        <v>6</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C105" s="10" t="str">
+        <f>C50</f>
+        <v>unique identifier</v>
+      </c>
+      <c r="D105" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C37, " - ", B39,")")</f>
         <v>Foreign key (QuanLy - IdQL)</v>
       </c>
-      <c r="E103" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F103" s="10" t="str">
-        <f>_xlfn.CONCAT(F39," (Quản lý duyệt)")</f>
-        <v>Id quản lý (Quản lý duyệt)</v>
-      </c>
-      <c r="G103" s="10"/>
-    </row>
-    <row r="104" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="23">
-        <v>4</v>
-      </c>
-      <c r="B104" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10"/>
-      <c r="F104" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G104" s="10"/>
-    </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A105" s="23">
-        <v>5</v>
-      </c>
-      <c r="B105" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10" t="s">
+      <c r="E105" s="10"/>
+      <c r="F105" s="10" t="str">
+        <f>_xlfn.CONCAT(F50," (Quản lý duyệt)")</f>
+        <v>Id tài khoản (Quản lý duyệt)</v>
+      </c>
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A106" s="23">
+        <v>7</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D106" s="27"/>
+      <c r="E106" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F105" s="10" t="s">
+      <c r="F106" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G106" s="10"/>
+    </row>
+    <row r="107" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A107" s="23">
+        <v>8</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G107" s="10"/>
+    </row>
+    <row r="108" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A108" s="23">
+        <v>9</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="23">
+        <v>10</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D109" s="27"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="G109" s="10"/>
+    </row>
+    <row r="110" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="23">
+        <v>11</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D110" s="27"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G110" s="10"/>
+    </row>
+    <row r="111" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A111" s="23">
+        <v>12</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G111" s="10"/>
+    </row>
+    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112" s="23">
+        <v>13</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F112" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B107" s="29"/>
-      <c r="C107" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D107" s="31"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="22"/>
-    </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A108" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G108" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A109" s="23">
-        <v>1</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D109" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E109" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="F109" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G109" s="10"/>
-    </row>
-    <row r="110" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A110" s="23">
-        <v>2</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C110" s="10" t="str">
-        <f>C83</f>
-        <v>varchar(15)</v>
-      </c>
-      <c r="D110" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C81, " - ", B83,")")</f>
-        <v>Foreign key (LopHoc - MaLH)</v>
-      </c>
-      <c r="E110" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F110" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A111" s="23">
-        <v>3</v>
-      </c>
-      <c r="B111" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C111" s="10" t="str">
-        <f>C94</f>
-        <v>varchar(10)</v>
-      </c>
-      <c r="D111" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C92, " - ", B94,")")</f>
-        <v>Foreign key (PhongHoc - MaPH)</v>
-      </c>
-      <c r="E111" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F111" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A112" s="23">
-        <v>4</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C112" s="10" t="str">
-        <f>C101</f>
-        <v>unique identifier</v>
-      </c>
-      <c r="D112" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C99, " - ", B101,")")</f>
-        <v>Foreign key (MuonPhongHoc - IdMPH)</v>
-      </c>
-      <c r="F112" s="10" t="str">
-        <f>F101</f>
-        <v>Id mượn phòng học</v>
-      </c>
-      <c r="G112" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G112" s="10"/>
+    </row>
+    <row r="113" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A113" s="23">
-        <v>5</v>
-      </c>
-      <c r="B113" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E113" s="10" t="s">
-        <v>16</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
       <c r="F113" s="10" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="G113" s="10"/>
     </row>
-    <row r="114" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="23">
-        <v>6</v>
-      </c>
-      <c r="B114" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C114" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F114" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G114" s="10"/>
-    </row>
-    <row r="115" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A115" s="23">
-        <v>7</v>
-      </c>
-      <c r="B115" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C115" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E115" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F115" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G115" s="10"/>
-    </row>
-    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="23">
-        <v>8</v>
-      </c>
-      <c r="B116" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F116" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G116" s="10"/>
-    </row>
-    <row r="117" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A117" s="23">
-        <v>9</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C117" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D117" s="10"/>
-      <c r="E117" s="10"/>
-      <c r="F117" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="G117" s="10"/>
-    </row>
-    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A118" s="24"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114" s="24"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
+  <mergeCells count="24">
     <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A107:B107"/>
     <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C107:D107"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A74:B74"/>
@@ -3365,6 +3286,18 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C81:D81"/>
     <mergeCell ref="C92:D92"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C47:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3389,14 +3322,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3548,14 +3481,14 @@
       <c r="A10" s="18"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3744,14 +3677,14 @@
       <c r="A22" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="30"/>
+      <c r="D23" s="29"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -3919,14 +3852,14 @@
       <c r="A33" s="18"/>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="30"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -4076,14 +4009,14 @@
       <c r="A43" s="18"/>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30" t="s">
+      <c r="B44" s="30"/>
+      <c r="C44" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="30"/>
+      <c r="D44" s="29"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -4145,14 +4078,14 @@
       <c r="A48" s="18"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="30" t="s">
+      <c r="B49" s="30"/>
+      <c r="C49" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="30"/>
+      <c r="D49" s="29"/>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -4214,14 +4147,14 @@
       <c r="A53" s="18"/>
     </row>
     <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="30" t="s">
+      <c r="B54" s="30"/>
+      <c r="C54" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D54" s="30"/>
+      <c r="D54" s="29"/>
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -4283,14 +4216,14 @@
       <c r="A58" s="18"/>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="30" t="s">
+      <c r="B59" s="30"/>
+      <c r="C59" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="30"/>
+      <c r="D59" s="29"/>
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -4391,14 +4324,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4549,14 +4482,14 @@
       <c r="A10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
@@ -4641,14 +4574,14 @@
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
     </row>
@@ -4747,14 +4680,14 @@
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
@@ -4879,14 +4812,14 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30" t="s">
+      <c r="B32" s="30"/>
+      <c r="C32" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="30"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
@@ -4985,14 +4918,14 @@
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="30" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="30"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
     </row>
@@ -5072,7 +5005,7 @@
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
         <v>4</v>
       </c>
@@ -5082,9 +5015,9 @@
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$99, " - ", 'Từ điển tổng hợp'!$B$101,")")</f>
-        <v>Foreign key (MuonPhongHoc - IdMPH)</v>
+      <c r="D44" s="10" t="e">
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!#REF!, " - ", 'Từ điển tổng hợp'!#REF!,")")</f>
+        <v>#REF!</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>74</v>
@@ -5170,18 +5103,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5207,14 +5140,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5370,14 +5303,14 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -5527,14 +5460,14 @@
       <c r="A20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
@@ -5659,14 +5592,14 @@
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="30"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
@@ -5766,14 +5699,14 @@
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="30" t="s">
+      <c r="B36" s="30"/>
+      <c r="C36" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
     </row>
@@ -5853,7 +5786,7 @@
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
         <v>4</v>
       </c>
@@ -5863,9 +5796,9 @@
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$99, " - ", 'Từ điển tổng hợp'!$B$101,")")</f>
-        <v>Foreign key (MuonPhongHoc - IdMPH)</v>
+      <c r="D41" s="10" t="e">
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!#REF!, " - ", 'Từ điển tổng hợp'!#REF!,")")</f>
+        <v>#REF!</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>74</v>
@@ -5950,10 +5883,10 @@
       <c r="A46" s="17"/>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="29"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="31" t="s">
         <v>89</v>
       </c>
@@ -6075,10 +6008,10 @@
       <c r="A54" s="17"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="29"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="31" t="s">
         <v>94</v>
       </c>
@@ -6163,7 +6096,7 @@
       </c>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A60" s="23">
         <v>4</v>
       </c>
@@ -6173,9 +6106,9 @@
       <c r="C60" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$99, " - ", 'Từ điển tổng hợp'!$B$101,")")</f>
-        <v>Foreign key (MuonPhongHoc - IdMPH)</v>
+      <c r="D60" s="10" t="e">
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!#REF!, " - ", 'Từ điển tổng hợp'!#REF!,")")</f>
+        <v>#REF!</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>74</v>
@@ -6265,10 +6198,10 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B66" s="29"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="31" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
update:     datebase fix:     model files name
</commit_message>
<xml_diff>
--- a/Từ điển dữ liệu.xlsx
+++ b/Từ điển dữ liệu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/746813123f077acb/Máy tính/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="529" documentId="13_ncr:1_{0E6CEDA0-CCDF-4949-A372-F8E2A066A992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB029229-56CE-4010-949E-F38A81353CA0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B3037B-89FD-43FE-808E-453A9F5A77DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="216">
   <si>
     <t>STT</t>
   </si>
@@ -655,9 +655,6 @@
     <t>varchar(10)</t>
   </si>
   <si>
-    <t>DsMPH</t>
-  </si>
-  <si>
     <t>MaLMPH</t>
   </si>
   <si>
@@ -686,6 +683,12 @@
   </si>
   <si>
     <t>tinyint</t>
+  </si>
+  <si>
+    <t>DsMPHLopHoc</t>
+  </si>
+  <si>
+    <t>DsMPHKhac</t>
   </si>
 </sst>
 </file>
@@ -920,13 +923,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1209,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C14DD0-095C-497D-B714-923494B6BFAC}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1227,14 +1230,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
@@ -1429,14 +1432,14 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="29" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
@@ -1578,7 +1581,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
@@ -1668,14 +1671,14 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
@@ -1793,7 +1796,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10" t="s">
@@ -1883,14 +1886,14 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="29" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="7"/>
       <c r="F37" s="17"/>
     </row>
@@ -2006,7 +2009,7 @@
         <v>26</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10" t="s">
@@ -2064,14 +2067,14 @@
       <c r="K46" s="26"/>
     </row>
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="29" t="s">
+      <c r="B47" s="29"/>
+      <c r="C47" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="D47" s="29"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="7"/>
       <c r="F47" s="17"/>
     </row>
@@ -2270,14 +2273,14 @@
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="30"/>
-      <c r="C58" s="29" t="s">
+      <c r="B58" s="29"/>
+      <c r="C58" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="29"/>
+      <c r="D58" s="31"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
     </row>
@@ -2355,14 +2358,14 @@
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="29" t="s">
+      <c r="B63" s="29"/>
+      <c r="C63" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="D63" s="29"/>
+      <c r="D63" s="31"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
     </row>
@@ -2430,14 +2433,14 @@
       <c r="G66" s="10"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
+      <c r="A68" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="30"/>
-      <c r="C68" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="D68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="D68" s="31"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
@@ -2472,18 +2475,18 @@
         <v>54</v>
       </c>
       <c r="C70" s="10" t="str">
-        <f>C83</f>
+        <f>C89</f>
         <v>varchar(15)</v>
       </c>
       <c r="D70" s="10" t="str">
-        <f>_xlfn.CONCAT("Primary key, Foreign key (",C81," - ",B83,")")</f>
+        <f>_xlfn.CONCAT("Primary key, Foreign key (",C87," - ",B89,")")</f>
         <v>Primary key, Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E70" s="28" t="s">
         <v>137</v>
       </c>
       <c r="F70" s="10" t="str">
-        <f>F83</f>
+        <f>F89</f>
         <v>Mã lớp học</v>
       </c>
       <c r="G70" s="10"/>
@@ -2531,23 +2534,15 @@
       </c>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-    </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="30"/>
-      <c r="C74" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="31"/>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
     </row>
@@ -2574,43 +2569,51 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A76" s="19">
         <v>1</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>123</v>
+        <v>204</v>
+      </c>
+      <c r="C76" s="10" t="str">
+        <f>C107</f>
+        <v>varchar(10)</v>
+      </c>
+      <c r="D76" s="10" t="str">
+        <f>_xlfn.CONCAT("Primary key, Foreign key (",C93," - ",B95,")")</f>
+        <v>Primary key, Foreign key (date - _CreateAt)</v>
       </c>
       <c r="E76" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F76" s="10" t="s">
-        <v>52</v>
+      <c r="F76" s="10" t="str">
+        <f>F107</f>
+        <v>Mã cấp phép mượn phòng học</v>
       </c>
       <c r="G76" s="10"/>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
         <v>2</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D77" s="27"/>
-      <c r="E77" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F77" s="10" t="s">
-        <v>53</v>
+        <v>165</v>
+      </c>
+      <c r="C77" s="10" t="str">
+        <f>C3</f>
+        <v>unique identifier</v>
+      </c>
+      <c r="D77" s="10" t="str">
+        <f>_xlfn.CONCAT("Primary key, Foreign key (",C7," - ",B9,")")</f>
+        <v>Primary key, Foreign key (varchar(30) - _UpdateAt)</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F77" s="10" t="str">
+        <f>_xlfn.CONCAT(F3, " (Tài khoản mượn phòng)")</f>
+        <v>Id tài khoản (Tài khoản mượn phòng)</v>
       </c>
       <c r="G77" s="10"/>
     </row>
@@ -2624,686 +2627,790 @@
       <c r="C78" s="10" t="s">
         <v>199</v>
       </c>
+      <c r="D78" s="10"/>
       <c r="E78" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F78" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A80" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="29"/>
+      <c r="C80" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="31"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="19">
+        <v>1</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E82" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A83" s="19">
+        <v>2</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D83" s="27"/>
+      <c r="E83" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A84" s="19">
+        <v>3</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G78" s="10"/>
-    </row>
-    <row r="79" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="19">
+      <c r="G84" s="10"/>
+    </row>
+    <row r="85" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A85" s="19">
         <v>4</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C85" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10" t="s">
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G79" s="10"/>
-    </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-    </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="30" t="s">
+      <c r="G85" s="10"/>
+    </row>
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="30"/>
-      <c r="C81" s="29" t="s">
+      <c r="B87" s="29"/>
+      <c r="C87" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="29"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-    </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+      <c r="D87" s="31"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D82" s="9" t="s">
+      <c r="B88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E88" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F82" s="9" t="s">
+      <c r="F88" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="G88" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A83" s="19">
-        <v>1</v>
-      </c>
-      <c r="B83" s="2" t="s">
+    <row r="89" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="19">
+        <v>1</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C89" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D83" s="10" t="s">
+      <c r="D89" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E83" s="28" t="s">
+      <c r="E89" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F89" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G83" s="10"/>
-    </row>
-    <row r="84" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="19">
-        <v>2</v>
-      </c>
-      <c r="B84" s="2" t="s">
+      <c r="G89" s="10"/>
+    </row>
+    <row r="90" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="19">
+        <v>2</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C84" s="10" t="str">
+      <c r="C90" s="10" t="str">
         <f>C3</f>
         <v>unique identifier</v>
       </c>
-      <c r="D84" s="10" t="str">
+      <c r="D90" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C25, " - ", B27,")")</f>
         <v>Foreign key (GiangVien - IdGV)</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E90" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F84" s="10" t="str">
+      <c r="F90" s="10" t="str">
         <f>_xlfn.CONCAT(F27, " (Giảng viên giảng dạy)")</f>
         <v>Id giảng viên (Giảng viên giảng dạy)</v>
       </c>
-      <c r="G84" s="10"/>
-    </row>
-    <row r="85" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="19">
+      <c r="G90" s="10"/>
+    </row>
+    <row r="91" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="19">
         <v>3</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C85" s="10" t="str">
-        <f>C76</f>
+      <c r="C91" s="10" t="str">
+        <f>C82</f>
         <v>varchar(15)</v>
       </c>
-      <c r="D85" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C74, " - ", B76,")")</f>
+      <c r="D91" s="10" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (", C80, " - ", B82,")")</f>
         <v>Foreign key (MonHoc - MaMH)</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E91" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F85" s="10" t="str">
-        <f>F76</f>
+      <c r="F91" s="10" t="str">
+        <f>F82</f>
         <v>Mã môn học</v>
       </c>
-      <c r="G85" s="10"/>
-    </row>
-    <row r="86" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="19">
+      <c r="G91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="19">
         <v>4</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C86" s="10" t="str">
+      <c r="C92" s="10" t="str">
         <f>C65</f>
         <v>varchar(20)</v>
       </c>
-      <c r="D86" s="10" t="str">
+      <c r="D92" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C63, " - ", B65,")")</f>
         <v>Foreign key (LopSV - MaLopSV)</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="E92" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="10" t="str">
+      <c r="F92" s="10" t="str">
         <f>_xlfn.CONCAT(F65, " (Lớp sinh viên giảng dạy)")</f>
         <v>Mã lớp sinh viên (Lớp sinh viên giảng dạy)</v>
       </c>
-      <c r="G86" s="10"/>
-    </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="19">
-        <v>5</v>
-      </c>
-      <c r="B87" s="2" t="s">
+      <c r="G92" s="10"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="19">
+        <v>5</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C93" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="10" t="s">
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="G87" s="10"/>
-    </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="19">
+      <c r="G93" s="10"/>
+    </row>
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A94" s="19">
         <v>6</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C94" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10" t="s">
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G88" s="10"/>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="19">
+      <c r="G94" s="10"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95" s="19">
         <v>7</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C95" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="D89" s="27"/>
-      <c r="E89" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G89" s="10"/>
-    </row>
-    <row r="90" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="19">
-        <v>8</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G90" s="10"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="21"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-    </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="B92" s="30"/>
-      <c r="C92" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D92" s="29"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="22"/>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="G93" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="19">
-        <v>1</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E94" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="F94" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="10"/>
-    </row>
-    <row r="95" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="19">
-        <v>2</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="D95" s="27"/>
       <c r="E95" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="G95" s="10"/>
     </row>
     <row r="96" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A96" s="19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A97" s="21"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+    </row>
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="29"/>
+      <c r="C98" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D98" s="31"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A100" s="19">
+        <v>1</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E100" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G100" s="10"/>
+    </row>
+    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="19">
+        <v>2</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" s="27"/>
+      <c r="E101" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="F101" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G101" s="10"/>
+    </row>
+    <row r="102" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A102" s="19">
+        <v>3</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F102" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G96" s="10"/>
-    </row>
-    <row r="97" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A97" s="19">
+      <c r="G102" s="10"/>
+    </row>
+    <row r="103" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="19">
         <v>4</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C103" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10" t="s">
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="G97" s="10"/>
-    </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-    </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="30" t="s">
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A104" s="18"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+    </row>
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B99" s="30"/>
-      <c r="C99" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="D99" s="31"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-    </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
+      <c r="B105" s="29"/>
+      <c r="C105" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="D105" s="30"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+    </row>
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B100" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D100" s="9" t="s">
+      <c r="B106" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E100" s="9" t="s">
+      <c r="E106" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F106" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G100" s="9" t="s">
+      <c r="G106" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A101" s="23">
-        <v>1</v>
-      </c>
-      <c r="B101" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C101" s="10" t="s">
+    <row r="107" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A107" s="23">
+        <v>1</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C107" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D101" s="10" t="s">
+      <c r="D107" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E101" s="28" t="s">
+      <c r="E107" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F101" s="10" t="s">
+      <c r="F107" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G101" s="10"/>
-    </row>
-    <row r="102" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="23">
-        <v>2</v>
-      </c>
-      <c r="B102" s="10" t="s">
+      <c r="G107" s="10"/>
+    </row>
+    <row r="108" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A108" s="23">
+        <v>2</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C102" s="10" t="str">
-        <f>C83</f>
+      <c r="C108" s="10" t="str">
+        <f>C89</f>
         <v>varchar(15)</v>
       </c>
-      <c r="D102" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C81, " - ", B83,")")</f>
+      <c r="D108" s="10" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (", C87, " - ", B89,")")</f>
         <v>Foreign key (LopHoc - MaLH)</v>
       </c>
-      <c r="E102" s="10" t="s">
+      <c r="E108" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F102" s="10" t="s">
+      <c r="F108" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G102" s="10"/>
-    </row>
-    <row r="103" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="23">
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="23">
         <v>3</v>
       </c>
-      <c r="B103" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C103" s="10" t="str">
-        <f>C94</f>
+      <c r="C109" s="10" t="str">
+        <f>C100</f>
         <v>varchar(10)</v>
       </c>
-      <c r="D103" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C92, " - ", B94,")")</f>
+      <c r="D109" s="10" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (", C98, " - ", B100,")")</f>
         <v>Foreign key (PhongHoc - MaPH)</v>
       </c>
-      <c r="E103" s="10" t="s">
+      <c r="E109" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F103" s="10" t="s">
+      <c r="F109" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G103" s="10"/>
-    </row>
-    <row r="104" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="23">
-        <v>5</v>
-      </c>
-      <c r="B104" s="10" t="s">
+      <c r="G109" s="10"/>
+    </row>
+    <row r="110" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A110" s="23">
+        <v>5</v>
+      </c>
+      <c r="B110" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C104" s="10" t="str">
+      <c r="C110" s="10" t="str">
         <f>C14</f>
         <v>unique identifier</v>
       </c>
-      <c r="D104" s="10" t="str">
+      <c r="D110" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (",C1, " - ", B3,")")</f>
         <v>Foreign key (TaiKhoan - IdTaiKhoan)</v>
       </c>
-      <c r="E104" s="10"/>
-      <c r="F104" s="10" t="s">
+      <c r="E110" s="10"/>
+      <c r="F110" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="G104" s="10"/>
-    </row>
-    <row r="105" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="23">
+      <c r="G110" s="10"/>
+    </row>
+    <row r="111" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A111" s="23">
         <v>6</v>
       </c>
-      <c r="B105" s="10" t="s">
+      <c r="B111" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C105" s="10" t="str">
+      <c r="C111" s="10" t="str">
         <f>C50</f>
         <v>unique identifier</v>
       </c>
-      <c r="D105" s="10" t="str">
+      <c r="D111" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C37, " - ", B39,")")</f>
         <v>Foreign key (QuanLy - IdQL)</v>
       </c>
-      <c r="E105" s="10"/>
-      <c r="F105" s="10" t="str">
+      <c r="E111" s="10"/>
+      <c r="F111" s="10" t="str">
         <f>_xlfn.CONCAT(F50," (Quản lý duyệt)")</f>
         <v>Id tài khoản (Quản lý duyệt)</v>
       </c>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A106" s="23">
+      <c r="G111" s="10"/>
+    </row>
+    <row r="112" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A112" s="23">
         <v>7</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B112" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D106" s="27"/>
-      <c r="E106" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F106" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G106" s="10"/>
-    </row>
-    <row r="107" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A107" s="23">
-        <v>8</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F107" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G107" s="10"/>
-    </row>
-    <row r="108" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A108" s="23">
-        <v>9</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F108" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="G108" s="10"/>
-    </row>
-    <row r="109" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="23">
-        <v>10</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D109" s="27"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="G109" s="10"/>
-    </row>
-    <row r="110" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A110" s="23">
-        <v>11</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D110" s="27"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A111" s="23">
-        <v>12</v>
-      </c>
-      <c r="B111" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C111" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A112" s="23">
-        <v>13</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D112" s="10"/>
+      <c r="D112" s="27"/>
       <c r="E112" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A113" s="23">
-        <v>14</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>161</v>
+        <v>8</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>199</v>
       </c>
       <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
+      <c r="E113" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F113" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="114" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A114" s="23">
+        <v>9</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F114" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G114" s="10"/>
+    </row>
+    <row r="115" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A115" s="23">
+        <v>10</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D115" s="27"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="G115" s="10"/>
+    </row>
+    <row r="116" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A116" s="23">
+        <v>11</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D116" s="27"/>
+      <c r="E116" s="10"/>
+      <c r="F116" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G116" s="10"/>
+    </row>
+    <row r="117" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A117" s="23">
+        <v>12</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="G117" s="10"/>
+    </row>
+    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A118" s="23">
+        <v>13</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F118" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G118" s="10"/>
+    </row>
+    <row r="119" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A119" s="23">
+        <v>14</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="24"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="G119" s="10"/>
+    </row>
+    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A120" s="24"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C92:D92"/>
+  <mergeCells count="26">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3328,14 +3435,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3487,14 +3594,14 @@
       <c r="A10" s="18"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3683,14 +3790,14 @@
       <c r="A22" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="29"/>
+      <c r="C23" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -3858,14 +3965,14 @@
       <c r="A33" s="18"/>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="29" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -4015,14 +4122,14 @@
       <c r="A43" s="18"/>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="29" t="s">
+      <c r="B44" s="29"/>
+      <c r="C44" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="29"/>
+      <c r="D44" s="31"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -4084,14 +4191,14 @@
       <c r="A48" s="18"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="29" t="s">
+      <c r="B49" s="29"/>
+      <c r="C49" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="29"/>
+      <c r="D49" s="31"/>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -4153,14 +4260,14 @@
       <c r="A53" s="18"/>
     </row>
     <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="29" t="s">
+      <c r="B54" s="29"/>
+      <c r="C54" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D54" s="29"/>
+      <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -4222,14 +4329,14 @@
       <c r="A58" s="18"/>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="29" t="s">
+      <c r="B59" s="29"/>
+      <c r="C59" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="29"/>
+      <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -4330,14 +4437,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4488,14 +4595,14 @@
       <c r="A10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
@@ -4580,14 +4687,14 @@
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
     </row>
@@ -4686,14 +4793,14 @@
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
@@ -4746,7 +4853,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$74, " - ", 'Từ điển tổng hợp'!$B$76,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$80, " - ", 'Từ điển tổng hợp'!$B$82,")")</f>
         <v>Foreign key (MonHoc - MaMH)</v>
       </c>
       <c r="E27" s="10" t="s">
@@ -4766,7 +4873,7 @@
       </c>
       <c r="D28" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$68, " - ", 'Từ điển tổng hợp'!$B$70,")")</f>
-        <v>Foreign key (DsMPH - MaLH)</v>
+        <v>Foreign key (DsMPHLopHoc - MaLH)</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>103</v>
@@ -4818,14 +4925,14 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="29" t="s">
+      <c r="B32" s="29"/>
+      <c r="C32" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
@@ -4924,14 +5031,14 @@
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="29"/>
+      <c r="C39" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="29"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
     </row>
@@ -4984,7 +5091,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$81, " - ", 'Từ điển tổng hợp'!$B$83,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$87, " - ", 'Từ điển tổng hợp'!$B$89,")")</f>
         <v>Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E42" s="10" t="s">
@@ -5003,7 +5110,7 @@
         <v>5</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$92, " - ", 'Từ điển tổng hợp'!$B$94,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$98, " - ", 'Từ điển tổng hợp'!$B$100,")")</f>
         <v>Foreign key (PhongHoc - MaPH)</v>
       </c>
       <c r="E43" s="10" t="s">
@@ -5109,18 +5216,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5146,14 +5253,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5309,14 +5416,14 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -5466,14 +5573,14 @@
       <c r="A20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="29" t="s">
+      <c r="B21" s="29"/>
+      <c r="C21" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
@@ -5526,7 +5633,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$74, " - ", 'Từ điển tổng hợp'!$B$76,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$80, " - ", 'Từ điển tổng hợp'!$B$82,")")</f>
         <v>Foreign key (MonHoc - MaMH)</v>
       </c>
       <c r="E24" s="10" t="s">
@@ -5546,7 +5653,7 @@
       </c>
       <c r="D25" s="10" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$68, " - ", 'Từ điển tổng hợp'!$B$70,")")</f>
-        <v>Foreign key (DsMPH - MaLH)</v>
+        <v>Foreign key (DsMPHLopHoc - MaLH)</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>103</v>
@@ -5598,14 +5705,14 @@
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
@@ -5705,14 +5812,14 @@
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="29" t="s">
+      <c r="B36" s="29"/>
+      <c r="C36" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="29"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
     </row>
@@ -5765,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$81, " - ", 'Từ điển tổng hợp'!$B$83,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$87, " - ", 'Từ điển tổng hợp'!$B$89,")")</f>
         <v>Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E39" s="10" t="s">
@@ -5784,7 +5891,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$92, " - ", 'Từ điển tổng hợp'!$B$94,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$98, " - ", 'Từ điển tổng hợp'!$B$100,")")</f>
         <v>Foreign key (PhongHoc - MaPH)</v>
       </c>
       <c r="E40" s="10" t="s">
@@ -5889,14 +5996,14 @@
       <c r="A46" s="17"/>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="31" t="s">
+      <c r="B47" s="29"/>
+      <c r="C47" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="31"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
@@ -6014,14 +6121,14 @@
       <c r="A54" s="17"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31" t="s">
+      <c r="B55" s="29"/>
+      <c r="C55" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="31"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
     </row>
@@ -6094,7 +6201,7 @@
         <v>5</v>
       </c>
       <c r="D59" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$92, " - ", 'Từ điển tổng hợp'!$B$94,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$98, " - ", 'Từ điển tổng hợp'!$B$100,")")</f>
         <v>Foreign key (PhongHoc - MaPH)</v>
       </c>
       <c r="E59" s="10" t="s">
@@ -6204,14 +6311,14 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B66" s="30"/>
-      <c r="C66" s="31" t="s">
+      <c r="B66" s="29"/>
+      <c r="C66" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D66" s="31"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
     </row>
@@ -6264,7 +6371,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$81, " - ", 'Từ điển tổng hợp'!$B$83,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$87, " - ", 'Từ điển tổng hợp'!$B$89,")")</f>
         <v>Foreign key (LopHoc - MaLH)</v>
       </c>
       <c r="E69" s="10" t="s">
@@ -6283,7 +6390,7 @@
         <v>5</v>
       </c>
       <c r="D70" s="10" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$92, " - ", 'Từ điển tổng hợp'!$B$94,")")</f>
+        <f>_xlfn.CONCAT( "Foreign key (", 'Từ điển tổng hợp'!$C$98, " - ", 'Từ điển tổng hợp'!$B$100,")")</f>
         <v>Foreign key (PhongHoc - MaPH)</v>
       </c>
       <c r="E70" s="10" t="s">

</xml_diff>

<commit_message>
update: models and beans. Fixed: database attributes
</commit_message>
<xml_diff>
--- a/Từ điển dữ liệu.xlsx
+++ b/Từ điển dữ liệu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A042B3-F1B8-4142-9871-3EF71C6CABB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E6020-B820-432A-A91E-88F82A0E574B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="195" windowWidth="14970" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="13800" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Từ điển tổng hợp" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="157">
   <si>
     <t>STT</t>
   </si>
@@ -315,15 +315,9 @@
     <t>_ExpireAt</t>
   </si>
   <si>
-    <t>Thời điểm hủy áp dụng (hủy môn học)</t>
-  </si>
-  <si>
     <t>Thời điểm hủy áp dụng (hủy lớp học)</t>
   </si>
   <si>
-    <t>Thời điểm hủy áp dụng (hủy phòng học)</t>
-  </si>
-  <si>
     <t>Thời điểm áp dụng</t>
   </si>
   <si>
@@ -499,6 +493,21 @@
   </si>
   <si>
     <t>IdNguoiDung</t>
+  </si>
+  <si>
+    <t>_DeactiveAt</t>
+  </si>
+  <si>
+    <t>Thời điểm hết hiệu lực (lớp học đã hoàn thành)</t>
+  </si>
+  <si>
+    <t>Ngăn thay đổi thông tin khi thuộc tính có dữ liệu.</t>
+  </si>
+  <si>
+    <t>Thời điểm hết hiệu lực (hủy mã và tên môn học)</t>
+  </si>
+  <si>
+    <t>Thời điểm hết hiệu lực (hủy trạng thái hoặc hủy phòng)</t>
   </si>
 </sst>
 </file>
@@ -692,13 +701,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C14DD0-095C-497D-B714-923494B6BFAC}">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -999,14 +1008,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="26"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
@@ -1024,7 +1033,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>50</v>
@@ -1041,10 +1050,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>53</v>
@@ -1059,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="9" t="str">
         <f>_xlfn.CONCAT( "Foreign Key (", C12, " - ", B14,", ",C24, " - ",B26, ", ", C35, " -  ",B37, ")")</f>
@@ -1072,7 +1081,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G4" s="9"/>
     </row>
@@ -1108,10 +1117,10 @@
         <v>67</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>53</v>
@@ -1120,7 +1129,7 @@
         <v>84</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1131,7 +1140,7 @@
         <v>68</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
@@ -1152,7 +1161,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
@@ -1171,17 +1180,17 @@
         <v>80</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1192,15 +1201,15 @@
         <v>81</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1212,14 +1221,14 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
@@ -1254,7 +1263,7 @@
         <v>71</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>51</v>
@@ -1299,10 +1308,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>53</v>
@@ -1320,10 +1329,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>53</v>
@@ -1341,10 +1350,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>53</v>
@@ -1365,7 +1374,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>53</v>
@@ -1383,7 +1392,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9" t="s">
@@ -1404,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
@@ -1414,7 +1423,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1425,7 +1434,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1443,14 +1452,14 @@
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
@@ -1485,7 +1494,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>51</v>
@@ -1506,10 +1515,10 @@
         <v>18</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>53</v>
@@ -1527,10 +1536,10 @@
         <v>8</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>53</v>
@@ -1548,10 +1557,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>53</v>
@@ -1572,7 +1581,7 @@
         <v>43</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>53</v>
@@ -1590,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
@@ -1611,7 +1620,7 @@
         <v>10</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9" t="s">
@@ -1621,7 +1630,7 @@
         <v>15</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1632,7 +1641,7 @@
         <v>72</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9" t="s">
@@ -1652,14 +1661,14 @@
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="24"/>
       <c r="E35" s="7"/>
       <c r="F35" s="14"/>
     </row>
@@ -1694,7 +1703,7 @@
         <v>47</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>51</v>
@@ -1712,19 +1721,19 @@
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G38" s="9"/>
     </row>
@@ -1736,10 +1745,10 @@
         <v>8</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>4</v>
@@ -1757,10 +1766,10 @@
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>4</v>
@@ -1781,7 +1790,7 @@
         <v>43</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>4</v>
@@ -1800,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9" t="s">
@@ -1821,7 +1830,7 @@
         <v>10</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9" t="s">
@@ -1831,7 +1840,7 @@
         <v>15</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1844,14 +1853,14 @@
       <c r="K44" s="21"/>
     </row>
     <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="26" t="s">
+      <c r="B45" s="25"/>
+      <c r="C45" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="26"/>
+      <c r="D45" s="24"/>
       <c r="E45" s="7"/>
       <c r="F45" s="14"/>
     </row>
@@ -1886,7 +1895,7 @@
         <v>76</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>51</v>
@@ -1902,10 +1911,10 @@
     <row r="48" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D48" s="9" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C35, " - ", B37,")")</f>
@@ -1915,7 +1924,7 @@
         <v>4</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G48" s="9"/>
     </row>
@@ -1927,7 +1936,7 @@
         <v>77</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9" t="s">
@@ -1946,7 +1955,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9" t="s">
@@ -1965,7 +1974,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
@@ -1984,12 +1993,12 @@
         <v>78</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G52" s="9"/>
     </row>
@@ -2001,17 +2010,17 @@
         <v>91</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K53" s="21"/>
     </row>
@@ -2024,14 +2033,14 @@
       <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="26" t="s">
+      <c r="B55" s="25"/>
+      <c r="C55" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="24"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
     </row>
@@ -2066,7 +2075,7 @@
         <v>65</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>51</v>
@@ -2087,10 +2096,10 @@
         <v>66</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>4</v>
@@ -2099,7 +2108,7 @@
         <v>20</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2111,14 +2120,14 @@
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="26"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="24"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
     </row>
@@ -2153,7 +2162,7 @@
         <v>41</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>51</v>
@@ -2171,13 +2180,13 @@
         <v>2</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>4</v>
@@ -2188,14 +2197,14 @@
       <c r="G63" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" s="26"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" s="24"/>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
     </row>
@@ -2227,20 +2236,20 @@
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D67" s="9" t="str">
-        <f>_xlfn.CONCAT("Primary Foreign Key (",C78," - ",B80, ", ",C97, " - ",B99,")")</f>
+        <f>_xlfn.CONCAT("Primary Foreign Key (",C78," - ",B80, ", ",C98, " - ",B100,")")</f>
         <v>Primary Foreign Key (LopHoc - MaLH, LichMuonPhong - MaLMPH)</v>
       </c>
       <c r="E67" s="23" t="s">
         <v>53</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G67" s="9"/>
     </row>
@@ -2249,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C68" s="9" t="str">
         <f>C3</f>
@@ -2263,7 +2272,7 @@
         <v>53</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G68" s="9"/>
     </row>
@@ -2275,7 +2284,7 @@
         <v>80</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9" t="s">
@@ -2285,18 +2294,18 @@
         <v>6</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="26" t="s">
+      <c r="B71" s="25"/>
+      <c r="C71" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D71" s="26"/>
+      <c r="D71" s="24"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
     </row>
@@ -2331,7 +2340,7 @@
         <v>21</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>51</v>
@@ -2352,7 +2361,7 @@
         <v>35</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9" t="s">
@@ -2363,43 +2372,43 @@
       </c>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="16">
         <v>3</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A76" s="16">
         <v>4</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2411,14 +2420,14 @@
       <c r="F77" s="7"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
+      <c r="A78" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="26" t="s">
+      <c r="B78" s="25"/>
+      <c r="C78" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D78" s="26"/>
+      <c r="D78" s="24"/>
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
     </row>
@@ -2453,7 +2462,7 @@
         <v>24</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>51</v>
@@ -2471,7 +2480,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C81" s="9" t="str">
         <f>C3</f>
@@ -2543,17 +2552,17 @@
         <v>5</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9" t="s">
         <v>59</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G84" s="9"/>
     </row>
@@ -2562,17 +2571,17 @@
         <v>6</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9" t="s">
         <v>59</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G85" s="9"/>
     </row>
@@ -2584,7 +2593,7 @@
         <v>79</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="9" t="s">
@@ -2603,16 +2612,16 @@
         <v>80</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
@@ -2623,558 +2632,567 @@
         <v>81</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="16">
+        <v>10</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="24" t="s">
+      <c r="A90" s="17"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A91" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B90" s="24"/>
-      <c r="C90" s="26" t="s">
+      <c r="B91" s="25"/>
+      <c r="C91" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D90" s="26"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="D91" s="24"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C92" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D92" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E92" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F92" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G91" s="8" t="s">
+      <c r="G92" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="16">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="16">
         <v>1</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D92" s="9" t="s">
+      <c r="C93" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D93" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E92" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F92" s="9" t="s">
+      <c r="E93" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F93" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="G92" s="9"/>
-    </row>
-    <row r="93" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="16">
-        <v>2</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="G93" s="9"/>
     </row>
     <row r="94" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A94" s="16">
+        <v>2</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G94" s="9"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95" s="16">
         <v>3</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G94" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="16">
-        <v>4</v>
-      </c>
       <c r="B95" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="F95" s="9" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="15"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-    </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="24" t="s">
+    <row r="96" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="16">
+        <v>4</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A97" s="15"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+    </row>
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B97" s="24"/>
-      <c r="C97" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D97" s="25"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-    </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A98" s="8" t="s">
+      <c r="B98" s="25"/>
+      <c r="C98" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D98" s="26"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A99" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B99" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C99" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D99" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="E99" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F98" s="8" t="s">
+      <c r="F99" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G98" s="8" t="s">
+      <c r="G99" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A99" s="19">
-        <v>1</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E99" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G99" s="9"/>
     </row>
     <row r="100" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A100" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C100" s="9" t="str">
-        <f>C92</f>
-        <v>varchar(7)</v>
-      </c>
-      <c r="D100" s="9" t="str">
-        <f>_xlfn.CONCAT( "Foreign key (", C90, " - ", B92,")")</f>
-        <v>Foreign key (PhongHoc - MaPH)</v>
-      </c>
-      <c r="E100" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E100" s="23" t="s">
         <v>53</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G100" s="9"/>
     </row>
     <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A101" s="19">
+        <v>2</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C101" s="9" t="str">
+        <f>C93</f>
+        <v>varchar(7)</v>
+      </c>
+      <c r="D101" s="9" t="str">
+        <f>_xlfn.CONCAT( "Foreign key (", C91, " - ", B93,")")</f>
+        <v>Foreign key (PhongHoc - MaPH)</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" s="9"/>
+    </row>
+    <row r="102" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A102" s="19">
         <v>3</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B102" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C101" s="9" t="str">
+      <c r="C102" s="9" t="str">
         <f>C80</f>
         <v>varchar(15)</v>
       </c>
-      <c r="D101" s="9" t="str">
+      <c r="D102" s="9" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C78, " - ", B80,")")</f>
         <v>Foreign key (LopHoc - MaLH)</v>
       </c>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G101" s="9"/>
-    </row>
-    <row r="102" spans="1:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="A102" s="19">
-        <v>4</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C102" s="9" t="str">
-        <f>C112</f>
-        <v>UUID</v>
-      </c>
-      <c r="D102" s="9" t="str">
-        <f>_xlfn.CONCAT( "Foreign Key (", C110, " - ", B112, ")")</f>
-        <v>Foreign Key (MuonPhongHoc - IdMPH)</v>
-      </c>
       <c r="E102" s="9"/>
       <c r="F102" s="9" t="s">
-        <v>147</v>
+        <v>25</v>
       </c>
       <c r="G102" s="9"/>
     </row>
-    <row r="103" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A103" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D103" s="22"/>
-      <c r="E103" s="9" t="s">
-        <v>4</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C103" s="9" t="str">
+        <f>C113</f>
+        <v>UUID</v>
+      </c>
+      <c r="D103" s="9" t="str">
+        <f>_xlfn.CONCAT( "Foreign Key (", C111, " - ", B113, ")")</f>
+        <v>Foreign Key (MuonPhongHoc - IdMPH)</v>
+      </c>
+      <c r="E103" s="9"/>
       <c r="F103" s="9" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="G103" s="9"/>
     </row>
     <row r="104" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A104" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D104" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="D104" s="22"/>
       <c r="E104" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G104" s="9"/>
     </row>
     <row r="105" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A105" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="D105" s="9"/>
       <c r="E105" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="G105" s="9"/>
     </row>
-    <row r="106" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A106" s="19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D106" s="22"/>
-      <c r="E106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="F106" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G106" s="9"/>
     </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A107" s="19">
+        <v>8</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D107" s="22"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G107" s="9"/>
+    </row>
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A108" s="19">
         <v>9</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B108" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F107" s="9" t="s">
+      <c r="C108" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G107" s="9"/>
-    </row>
-    <row r="108" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="19">
+      <c r="G108" s="9"/>
+    </row>
+    <row r="109" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="19">
         <v>10</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C108" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G108" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A109" s="20"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="10"/>
-    </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="24" t="s">
+      <c r="C109" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A110" s="20"/>
+      <c r="B110" s="10"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+    </row>
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="D110" s="25"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-    </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A111" s="8" t="s">
+      <c r="B111" s="25"/>
+      <c r="C111" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D111" s="26"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+    </row>
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B112" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="8" t="s">
+      <c r="C112" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D111" s="8" t="s">
+      <c r="D112" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="E112" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F111" s="8" t="s">
+      <c r="F112" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G111" s="8" t="s">
+      <c r="G112" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A112" s="19">
+    <row r="113" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A113" s="19">
         <v>1</v>
       </c>
-      <c r="B112" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C112" s="9" t="s">
+      <c r="B113" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E113" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G113" s="9"/>
+    </row>
+    <row r="114" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="A114" s="19">
+        <v>2</v>
+      </c>
+      <c r="B114" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D112" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E112" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G112" s="9"/>
-    </row>
-    <row r="113" spans="1:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="A113" s="19">
-        <v>2</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D113" s="9" t="str">
+      <c r="C114" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="9" t="str">
         <f>_xlfn.CONCAT( "Foreign Key (", C12, " - ", B14,", ",C24, " - ",B26, ", ", C35, " -  ",B37, ")")</f>
         <v>Foreign Key (SinhVien - IdSV, GiangVien - IdGV, QuanLy -  IdQL)</v>
       </c>
-      <c r="E113" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G113" s="9"/>
-    </row>
-    <row r="114" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="19">
+      <c r="E114" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G114" s="9"/>
+    </row>
+    <row r="115" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A115" s="19">
         <v>3</v>
       </c>
-      <c r="B114" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C114" s="9" t="str">
+      <c r="B115" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C115" s="9" t="str">
         <f>C37</f>
         <v>UUID</v>
       </c>
-      <c r="D114" s="9" t="str">
+      <c r="D115" s="9" t="str">
         <f>_xlfn.CONCAT( "Foreign key (", C35, " - ", B37,")")</f>
         <v>Foreign key (QuanLy - IdQL)</v>
       </c>
-      <c r="E114" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G114" s="9"/>
-    </row>
-    <row r="115" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A115" s="19">
-        <v>4</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D115" s="22"/>
       <c r="E115" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="G115" s="9"/>
     </row>
     <row r="116" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A116" s="19">
+        <v>4</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D116" s="22"/>
+      <c r="E116" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G116" s="9"/>
+    </row>
+    <row r="117" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A117" s="19">
         <v>5</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B117" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C116" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D116" s="9"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G116" s="9"/>
-    </row>
-    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A117" s="19">
+      <c r="C117" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G117" s="9"/>
+    </row>
+    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A118" s="19">
         <v>6</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B118" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C117" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D117" s="9"/>
-      <c r="E117" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F117" s="9" t="s">
+      <c r="C118" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F118" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G117" s="9"/>
+      <c r="G118" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="C111:D111"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C24:D24"/>
@@ -3187,8 +3205,18 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C91:D91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3221,7 +3249,7 @@
         <v>79</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9" t="s">
@@ -3240,17 +3268,17 @@
         <v>80</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -3261,15 +3289,15 @@
         <v>81</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>